<commit_message>
added referee stats and finalspreads
</commit_message>
<xml_diff>
--- a/Squads/F1/Clermont_Lyon_squad.xlsx
+++ b/Squads/F1/Clermont_Lyon_squad.xlsx
@@ -90,97 +90,97 @@
     <t>Aer%</t>
   </si>
   <si>
-    <t>2361</t>
-  </si>
-  <si>
-    <t>1531</t>
-  </si>
-  <si>
-    <t>2415</t>
-  </si>
-  <si>
-    <t>1779</t>
-  </si>
-  <si>
-    <t>1793</t>
-  </si>
-  <si>
-    <t>1297</t>
-  </si>
-  <si>
-    <t>86</t>
-  </si>
-  <si>
-    <t>255</t>
-  </si>
-  <si>
-    <t>395</t>
-  </si>
-  <si>
-    <t>654</t>
-  </si>
-  <si>
-    <t>669</t>
-  </si>
-  <si>
-    <t>1039</t>
-  </si>
-  <si>
-    <t>1310</t>
-  </si>
-  <si>
-    <t>1411</t>
-  </si>
-  <si>
-    <t>1536</t>
-  </si>
-  <si>
-    <t>53</t>
-  </si>
-  <si>
-    <t>422</t>
-  </si>
-  <si>
-    <t>1362</t>
-  </si>
-  <si>
-    <t>1459</t>
-  </si>
-  <si>
-    <t>1665</t>
-  </si>
-  <si>
-    <t>1842</t>
-  </si>
-  <si>
-    <t>2158</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>131</t>
-  </si>
-  <si>
-    <t>483</t>
+    <t>2385</t>
+  </si>
+  <si>
+    <t>1547</t>
+  </si>
+  <si>
+    <t>2439</t>
+  </si>
+  <si>
+    <t>1797</t>
+  </si>
+  <si>
+    <t>1811</t>
+  </si>
+  <si>
+    <t>1309</t>
+  </si>
+  <si>
+    <t>87</t>
+  </si>
+  <si>
+    <t>258</t>
+  </si>
+  <si>
+    <t>399</t>
+  </si>
+  <si>
+    <t>661</t>
   </si>
   <si>
     <t>676</t>
   </si>
   <si>
-    <t>821</t>
-  </si>
-  <si>
-    <t>1139</t>
-  </si>
-  <si>
-    <t>1397</t>
-  </si>
-  <si>
-    <t>2075</t>
-  </si>
-  <si>
-    <t>2192</t>
+    <t>1047</t>
+  </si>
+  <si>
+    <t>1322</t>
+  </si>
+  <si>
+    <t>1423</t>
+  </si>
+  <si>
+    <t>1552</t>
+  </si>
+  <si>
+    <t>1860</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>426</t>
+  </si>
+  <si>
+    <t>1374</t>
+  </si>
+  <si>
+    <t>1472</t>
+  </si>
+  <si>
+    <t>1681</t>
+  </si>
+  <si>
+    <t>2180</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>133</t>
+  </si>
+  <si>
+    <t>488</t>
+  </si>
+  <si>
+    <t>683</t>
+  </si>
+  <si>
+    <t>828</t>
+  </si>
+  <si>
+    <t>1148</t>
+  </si>
+  <si>
+    <t>1409</t>
+  </si>
+  <si>
+    <t>2096</t>
+  </si>
+  <si>
+    <t>2214</t>
   </si>
   <si>
     <t>Nicolás Tagliafico</t>
@@ -228,6 +228,9 @@
     <t>Nemanja Matić</t>
   </si>
   <si>
+    <t>Gift Orban</t>
+  </si>
+  <si>
     <t>Paul Akouokou</t>
   </si>
   <si>
@@ -243,9 +246,6 @@
     <t>Diego Moreira</t>
   </si>
   <si>
-    <t>Gift Orban</t>
-  </si>
-  <si>
     <t>Mama Samba Baldé</t>
   </si>
   <si>
@@ -306,15 +306,15 @@
     <t>rs SRB</t>
   </si>
   <si>
+    <t>ng NGA</t>
+  </si>
+  <si>
     <t>eng ENG</t>
   </si>
   <si>
     <t>pt POR</t>
   </si>
   <si>
-    <t>ng NGA</t>
-  </si>
-  <si>
     <t>gw GNB</t>
   </si>
   <si>
@@ -351,97 +351,97 @@
     <t>fr Ligue 1</t>
   </si>
   <si>
-    <t>31-250</t>
-  </si>
-  <si>
-    <t>31-182</t>
-  </si>
-  <si>
-    <t>29-278</t>
-  </si>
-  <si>
-    <t>20-188</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>19-042</t>
-  </si>
-  <si>
-    <t>22-003</t>
-  </si>
-  <si>
-    <t>28-271</t>
-  </si>
-  <si>
-    <t>27-233</t>
-  </si>
-  <si>
-    <t>19-080</t>
-  </si>
-  <si>
-    <t>23-028</t>
-  </si>
-  <si>
-    <t>30-012</t>
-  </si>
-  <si>
-    <t>32-345</t>
-  </si>
-  <si>
-    <t>34-307</t>
-  </si>
-  <si>
-    <t>35-280</t>
-  </si>
-  <si>
-    <t>26-139</t>
-  </si>
-  <si>
-    <t>24-082</t>
-  </si>
-  <si>
-    <t>21-198</t>
-  </si>
-  <si>
-    <t>26-252</t>
-  </si>
-  <si>
-    <t>19-275</t>
-  </si>
-  <si>
-    <t>21-295</t>
-  </si>
-  <si>
-    <t>28-183</t>
-  </si>
-  <si>
-    <t>26-045</t>
-  </si>
-  <si>
-    <t>20-031</t>
-  </si>
-  <si>
-    <t>20-264</t>
-  </si>
-  <si>
-    <t>20-090</t>
-  </si>
-  <si>
-    <t>19-037</t>
-  </si>
-  <si>
-    <t>24-129</t>
-  </si>
-  <si>
-    <t>33-219</t>
-  </si>
-  <si>
-    <t>36-275</t>
-  </si>
-  <si>
-    <t>18-252</t>
+    <t>31-262</t>
+  </si>
+  <si>
+    <t>31-194</t>
+  </si>
+  <si>
+    <t>29-290</t>
+  </si>
+  <si>
+    <t>20-200</t>
+  </si>
+  <si>
+    <t>23-004</t>
+  </si>
+  <si>
+    <t>19-054</t>
+  </si>
+  <si>
+    <t>22-015</t>
+  </si>
+  <si>
+    <t>28-283</t>
+  </si>
+  <si>
+    <t>27-245</t>
+  </si>
+  <si>
+    <t>19-092</t>
+  </si>
+  <si>
+    <t>23-040</t>
+  </si>
+  <si>
+    <t>30-024</t>
+  </si>
+  <si>
+    <t>32-357</t>
+  </si>
+  <si>
+    <t>34-319</t>
+  </si>
+  <si>
+    <t>35-292</t>
+  </si>
+  <si>
+    <t>21-307</t>
+  </si>
+  <si>
+    <t>26-151</t>
+  </si>
+  <si>
+    <t>24-094</t>
+  </si>
+  <si>
+    <t>21-210</t>
+  </si>
+  <si>
+    <t>26-264</t>
+  </si>
+  <si>
+    <t>19-287</t>
+  </si>
+  <si>
+    <t>28-195</t>
+  </si>
+  <si>
+    <t>26-057</t>
+  </si>
+  <si>
+    <t>20-043</t>
+  </si>
+  <si>
+    <t>20-276</t>
+  </si>
+  <si>
+    <t>20-102</t>
+  </si>
+  <si>
+    <t>19-049</t>
+  </si>
+  <si>
+    <t>24-141</t>
+  </si>
+  <si>
+    <t>33-231</t>
+  </si>
+  <si>
+    <t>36-287</t>
+  </si>
+  <si>
+    <t>18-264</t>
   </si>
   <si>
     <t>1992</t>
@@ -453,6 +453,9 @@
     <t>2003</t>
   </si>
   <si>
+    <t>2001</t>
+  </si>
+  <si>
     <t>2005</t>
   </si>
   <si>
@@ -463,9 +466,6 @@
   </si>
   <si>
     <t>1996</t>
-  </si>
-  <si>
-    <t>2001</t>
   </si>
   <si>
     <t>1991</t>
@@ -701,7 +701,7 @@
         <v>25</v>
       </c>
       <c r="B2" t="n">
-        <v>2490.0</v>
+        <v>2514.0</v>
       </c>
       <c r="C2" t="s">
         <v>56</v>
@@ -740,7 +740,7 @@
         <v>35.0</v>
       </c>
       <c r="O2" t="n">
-        <v>30.0</v>
+        <v>31.0</v>
       </c>
       <c r="P2" t="n">
         <v>0.0</v>
@@ -749,10 +749,10 @@
         <v>36.0</v>
       </c>
       <c r="R2" t="n">
-        <v>23.0</v>
+        <v>24.0</v>
       </c>
       <c r="S2" t="n">
-        <v>33.0</v>
+        <v>34.0</v>
       </c>
       <c r="T2" t="n">
         <v>1.0</v>
@@ -764,7 +764,7 @@
         <v>0.0</v>
       </c>
       <c r="W2" t="n">
-        <v>71.0</v>
+        <v>73.0</v>
       </c>
       <c r="X2" t="n">
         <v>19.0</v>
@@ -781,7 +781,7 @@
         <v>26</v>
       </c>
       <c r="B3" t="n">
-        <v>1620.0</v>
+        <v>1636.0</v>
       </c>
       <c r="C3" t="s">
         <v>57</v>
@@ -805,10 +805,10 @@
         <v>143</v>
       </c>
       <c r="J3" t="n">
-        <v>22.7</v>
+        <v>23.7</v>
       </c>
       <c r="K3" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="L3" t="n">
         <v>0.0</v>
@@ -817,22 +817,22 @@
         <v>0.0</v>
       </c>
       <c r="N3" t="n">
-        <v>24.0</v>
+        <v>29.0</v>
       </c>
       <c r="O3" t="n">
-        <v>35.0</v>
+        <v>36.0</v>
       </c>
       <c r="P3" t="n">
         <v>1.0</v>
       </c>
       <c r="Q3" t="n">
-        <v>41.0</v>
+        <v>48.0</v>
       </c>
       <c r="R3" t="n">
-        <v>36.0</v>
+        <v>40.0</v>
       </c>
       <c r="S3" t="n">
-        <v>21.0</v>
+        <v>22.0</v>
       </c>
       <c r="T3" t="n">
         <v>0.0</v>
@@ -844,16 +844,16 @@
         <v>0.0</v>
       </c>
       <c r="W3" t="n">
-        <v>130.0</v>
+        <v>139.0</v>
       </c>
       <c r="X3" t="n">
-        <v>24.0</v>
+        <v>26.0</v>
       </c>
       <c r="Y3" t="n">
-        <v>26.0</v>
+        <v>27.0</v>
       </c>
       <c r="Z3" t="n">
-        <v>48.0</v>
+        <v>49.1</v>
       </c>
     </row>
     <row r="4">
@@ -861,7 +861,7 @@
         <v>27</v>
       </c>
       <c r="B4" t="n">
-        <v>2545.0</v>
+        <v>2569.0</v>
       </c>
       <c r="C4" t="s">
         <v>58</v>
@@ -903,16 +903,16 @@
         <v>21.0</v>
       </c>
       <c r="P4" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="Q4" t="n">
-        <v>32.0</v>
+        <v>35.0</v>
       </c>
       <c r="R4" t="n">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="S4" t="n">
-        <v>19.0</v>
+        <v>20.0</v>
       </c>
       <c r="T4" t="n">
         <v>0.0</v>
@@ -924,16 +924,16 @@
         <v>0.0</v>
       </c>
       <c r="W4" t="n">
-        <v>115.0</v>
+        <v>116.0</v>
       </c>
       <c r="X4" t="n">
         <v>36.0</v>
       </c>
       <c r="Y4" t="n">
-        <v>21.0</v>
+        <v>22.0</v>
       </c>
       <c r="Z4" t="n">
-        <v>63.2</v>
+        <v>62.1</v>
       </c>
     </row>
     <row r="5">
@@ -941,7 +941,7 @@
         <v>28</v>
       </c>
       <c r="B5" t="n">
-        <v>1881.0</v>
+        <v>1899.0</v>
       </c>
       <c r="C5" t="s">
         <v>59</v>
@@ -965,7 +965,7 @@
         <v>145</v>
       </c>
       <c r="J5" t="n">
-        <v>19.9</v>
+        <v>20.2</v>
       </c>
       <c r="K5" t="n">
         <v>4.0</v>
@@ -977,22 +977,22 @@
         <v>0.0</v>
       </c>
       <c r="N5" t="n">
-        <v>47.0</v>
+        <v>49.0</v>
       </c>
       <c r="O5" t="n">
-        <v>28.0</v>
+        <v>33.0</v>
       </c>
       <c r="P5" t="n">
         <v>12.0</v>
       </c>
       <c r="Q5" t="n">
-        <v>71.0</v>
+        <v>75.0</v>
       </c>
       <c r="R5" t="n">
         <v>8.0</v>
       </c>
       <c r="S5" t="n">
-        <v>12.0</v>
+        <v>14.0</v>
       </c>
       <c r="T5" t="n">
         <v>0.0</v>
@@ -1004,16 +1004,16 @@
         <v>0.0</v>
       </c>
       <c r="W5" t="n">
-        <v>78.0</v>
+        <v>83.0</v>
       </c>
       <c r="X5" t="n">
         <v>10.0</v>
       </c>
       <c r="Y5" t="n">
-        <v>24.0</v>
+        <v>25.0</v>
       </c>
       <c r="Z5" t="n">
-        <v>29.4</v>
+        <v>28.6</v>
       </c>
     </row>
     <row r="6">
@@ -1021,7 +1021,7 @@
         <v>29</v>
       </c>
       <c r="B6" t="n">
-        <v>1896.0</v>
+        <v>1914.0</v>
       </c>
       <c r="C6" t="s">
         <v>60</v>
@@ -1042,10 +1042,10 @@
         <v>116</v>
       </c>
       <c r="I6" t="s">
-        <v>116</v>
+        <v>146</v>
       </c>
       <c r="J6" t="n">
-        <v>24.3</v>
+        <v>25.3</v>
       </c>
       <c r="K6" t="n">
         <v>4.0</v>
@@ -1060,7 +1060,7 @@
         <v>17.0</v>
       </c>
       <c r="O6" t="n">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="P6" t="n">
         <v>0.0</v>
@@ -1069,10 +1069,10 @@
         <v>1.0</v>
       </c>
       <c r="R6" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
       <c r="S6" t="n">
-        <v>14.0</v>
+        <v>15.0</v>
       </c>
       <c r="T6" t="n">
         <v>0.0</v>
@@ -1084,16 +1084,16 @@
         <v>0.0</v>
       </c>
       <c r="W6" t="n">
-        <v>117.0</v>
+        <v>123.0</v>
       </c>
       <c r="X6" t="n">
-        <v>38.0</v>
+        <v>41.0</v>
       </c>
       <c r="Y6" t="n">
-        <v>20.0</v>
+        <v>25.0</v>
       </c>
       <c r="Z6" t="n">
-        <v>65.5</v>
+        <v>62.1</v>
       </c>
     </row>
     <row r="7">
@@ -1101,7 +1101,7 @@
         <v>30</v>
       </c>
       <c r="B7" t="n">
-        <v>1373.0</v>
+        <v>1385.0</v>
       </c>
       <c r="C7" t="s">
         <v>61</v>
@@ -1122,7 +1122,7 @@
         <v>117</v>
       </c>
       <c r="I7" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="J7" t="n">
         <v>10.3</v>
@@ -1181,7 +1181,7 @@
         <v>31</v>
       </c>
       <c r="B8" t="n">
-        <v>91.0</v>
+        <v>92.0</v>
       </c>
       <c r="C8" t="s">
         <v>62</v>
@@ -1202,7 +1202,7 @@
         <v>118</v>
       </c>
       <c r="I8" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J8" t="n">
         <v>4.7</v>
@@ -1261,7 +1261,7 @@
         <v>32</v>
       </c>
       <c r="B9" t="n">
-        <v>275.0</v>
+        <v>278.0</v>
       </c>
       <c r="C9" t="s">
         <v>63</v>
@@ -1270,7 +1270,7 @@
         <v>92</v>
       </c>
       <c r="E9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F9" t="s">
         <v>110</v>
@@ -1282,7 +1282,7 @@
         <v>119</v>
       </c>
       <c r="I9" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="J9" t="n">
         <v>7.8</v>
@@ -1303,10 +1303,10 @@
         <v>10.0</v>
       </c>
       <c r="P9" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="Q9" t="n">
-        <v>60.0</v>
+        <v>65.0</v>
       </c>
       <c r="R9" t="n">
         <v>1.0</v>
@@ -1324,7 +1324,7 @@
         <v>0.0</v>
       </c>
       <c r="W9" t="n">
-        <v>35.0</v>
+        <v>38.0</v>
       </c>
       <c r="X9" t="n">
         <v>1.0</v>
@@ -1341,7 +1341,7 @@
         <v>33</v>
       </c>
       <c r="B10" t="n">
-        <v>423.0</v>
+        <v>427.0</v>
       </c>
       <c r="C10" t="s">
         <v>64</v>
@@ -1362,10 +1362,10 @@
         <v>120</v>
       </c>
       <c r="I10" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="J10" t="n">
-        <v>20.1</v>
+        <v>21.1</v>
       </c>
       <c r="K10" t="n">
         <v>2.0</v>
@@ -1380,7 +1380,7 @@
         <v>16.0</v>
       </c>
       <c r="O10" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="P10" t="n">
         <v>0.0</v>
@@ -1389,10 +1389,10 @@
         <v>0.0</v>
       </c>
       <c r="R10" t="n">
-        <v>13.0</v>
+        <v>17.0</v>
       </c>
       <c r="S10" t="n">
-        <v>9.0</v>
+        <v>11.0</v>
       </c>
       <c r="T10" t="n">
         <v>0.0</v>
@@ -1404,16 +1404,16 @@
         <v>0.0</v>
       </c>
       <c r="W10" t="n">
-        <v>73.0</v>
+        <v>83.0</v>
       </c>
       <c r="X10" t="n">
-        <v>43.0</v>
+        <v>51.0</v>
       </c>
       <c r="Y10" t="n">
-        <v>14.0</v>
+        <v>15.0</v>
       </c>
       <c r="Z10" t="n">
-        <v>75.4</v>
+        <v>77.3</v>
       </c>
     </row>
     <row r="11">
@@ -1421,7 +1421,7 @@
         <v>34</v>
       </c>
       <c r="B11" t="n">
-        <v>692.0</v>
+        <v>699.0</v>
       </c>
       <c r="C11" t="s">
         <v>65</v>
@@ -1442,10 +1442,10 @@
         <v>121</v>
       </c>
       <c r="I11" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="J11" t="n">
-        <v>3.9</v>
+        <v>4.0</v>
       </c>
       <c r="K11" t="n">
         <v>2.0</v>
@@ -1472,7 +1472,7 @@
         <v>4.0</v>
       </c>
       <c r="S11" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="T11" t="n">
         <v>0.0</v>
@@ -1484,7 +1484,7 @@
         <v>0.0</v>
       </c>
       <c r="W11" t="n">
-        <v>17.0</v>
+        <v>18.0</v>
       </c>
       <c r="X11" t="n">
         <v>3.0</v>
@@ -1501,7 +1501,7 @@
         <v>35</v>
       </c>
       <c r="B12" t="n">
-        <v>708.0</v>
+        <v>715.0</v>
       </c>
       <c r="C12" t="s">
         <v>66</v>
@@ -1522,7 +1522,7 @@
         <v>122</v>
       </c>
       <c r="I12" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="J12" t="n">
         <v>9.9</v>
@@ -1581,7 +1581,7 @@
         <v>36</v>
       </c>
       <c r="B13" t="n">
-        <v>1099.0</v>
+        <v>1107.0</v>
       </c>
       <c r="C13" t="s">
         <v>67</v>
@@ -1605,7 +1605,7 @@
         <v>144</v>
       </c>
       <c r="J13" t="n">
-        <v>5.9</v>
+        <v>6.7</v>
       </c>
       <c r="K13" t="n">
         <v>2.0</v>
@@ -1626,31 +1626,31 @@
         <v>0.0</v>
       </c>
       <c r="Q13" t="n">
-        <v>16.0</v>
+        <v>17.0</v>
       </c>
       <c r="R13" t="n">
         <v>10.0</v>
       </c>
       <c r="S13" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="T13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V13" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W13" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="X13" t="n">
         <v>5.0</v>
       </c>
-      <c r="T13" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="U13" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="V13" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="W13" t="n">
-        <v>22.0</v>
-      </c>
-      <c r="X13" t="n">
-        <v>4.0</v>
-      </c>
       <c r="Y13" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="Z13" t="n">
         <v>50.0</v>
@@ -1661,7 +1661,7 @@
         <v>37</v>
       </c>
       <c r="B14" t="n">
-        <v>1386.0</v>
+        <v>1398.0</v>
       </c>
       <c r="C14" t="s">
         <v>68</v>
@@ -1685,7 +1685,7 @@
         <v>151</v>
       </c>
       <c r="J14" t="n">
-        <v>24.3</v>
+        <v>24.5</v>
       </c>
       <c r="K14" t="n">
         <v>2.0</v>
@@ -1697,13 +1697,13 @@
         <v>0.0</v>
       </c>
       <c r="N14" t="n">
-        <v>48.0</v>
+        <v>49.0</v>
       </c>
       <c r="O14" t="n">
-        <v>35.0</v>
+        <v>36.0</v>
       </c>
       <c r="P14" t="n">
-        <v>12.0</v>
+        <v>13.0</v>
       </c>
       <c r="Q14" t="n">
         <v>10.0</v>
@@ -1724,16 +1724,16 @@
         <v>0.0</v>
       </c>
       <c r="W14" t="n">
-        <v>56.0</v>
+        <v>59.0</v>
       </c>
       <c r="X14" t="n">
-        <v>25.0</v>
+        <v>26.0</v>
       </c>
       <c r="Y14" t="n">
         <v>39.0</v>
       </c>
       <c r="Z14" t="n">
-        <v>39.1</v>
+        <v>40.0</v>
       </c>
     </row>
     <row r="15">
@@ -1741,7 +1741,7 @@
         <v>38</v>
       </c>
       <c r="B15" t="n">
-        <v>1492.0</v>
+        <v>1504.0</v>
       </c>
       <c r="C15" t="s">
         <v>69</v>
@@ -1821,7 +1821,7 @@
         <v>39</v>
       </c>
       <c r="B16" t="n">
-        <v>1626.0</v>
+        <v>1642.0</v>
       </c>
       <c r="C16" t="s">
         <v>70</v>
@@ -1845,7 +1845,7 @@
         <v>153</v>
       </c>
       <c r="J16" t="n">
-        <v>12.1</v>
+        <v>12.9</v>
       </c>
       <c r="K16" t="n">
         <v>2.0</v>
@@ -1857,7 +1857,7 @@
         <v>0.0</v>
       </c>
       <c r="N16" t="n">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="O16" t="n">
         <v>8.0</v>
@@ -1866,10 +1866,10 @@
         <v>0.0</v>
       </c>
       <c r="Q16" t="n">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="R16" t="n">
-        <v>15.0</v>
+        <v>16.0</v>
       </c>
       <c r="S16" t="n">
         <v>10.0</v>
@@ -1884,16 +1884,16 @@
         <v>1.0</v>
       </c>
       <c r="W16" t="n">
-        <v>92.0</v>
+        <v>98.0</v>
       </c>
       <c r="X16" t="n">
-        <v>17.0</v>
+        <v>19.0</v>
       </c>
       <c r="Y16" t="n">
         <v>9.0</v>
       </c>
       <c r="Z16" t="n">
-        <v>65.4</v>
+        <v>67.9</v>
       </c>
     </row>
     <row r="17">
@@ -1901,16 +1901,16 @@
         <v>40</v>
       </c>
       <c r="B17" t="n">
-        <v>57.0</v>
+        <v>1964.0</v>
       </c>
       <c r="C17" t="s">
         <v>71</v>
       </c>
       <c r="D17" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="E17" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F17" t="s">
         <v>110</v>
@@ -1922,13 +1922,13 @@
         <v>127</v>
       </c>
       <c r="I17" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="J17" t="n">
-        <v>3.4</v>
+        <v>5.3</v>
       </c>
       <c r="K17" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="L17" t="n">
         <v>0.0</v>
@@ -1940,19 +1940,19 @@
         <v>9.0</v>
       </c>
       <c r="O17" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="P17" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="Q17" t="n">
         <v>3.0</v>
       </c>
-      <c r="P17" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Q17" t="n">
-        <v>0.0</v>
-      </c>
       <c r="R17" t="n">
-        <v>6.0</v>
+        <v>1.0</v>
       </c>
       <c r="S17" t="n">
-        <v>9.0</v>
+        <v>3.0</v>
       </c>
       <c r="T17" t="n">
         <v>0.0</v>
@@ -1964,16 +1964,16 @@
         <v>0.0</v>
       </c>
       <c r="W17" t="n">
-        <v>25.0</v>
+        <v>14.0</v>
       </c>
       <c r="X17" t="n">
-        <v>8.0</v>
+        <v>3.0</v>
       </c>
       <c r="Y17" t="n">
-        <v>5.0</v>
+        <v>15.0</v>
       </c>
       <c r="Z17" t="n">
-        <v>61.5</v>
+        <v>16.7</v>
       </c>
     </row>
     <row r="18">
@@ -1981,13 +1981,13 @@
         <v>41</v>
       </c>
       <c r="B18" t="n">
-        <v>450.0</v>
+        <v>58.0</v>
       </c>
       <c r="C18" t="s">
         <v>72</v>
       </c>
       <c r="D18" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="E18" t="s">
         <v>104</v>
@@ -2002,10 +2002,10 @@
         <v>128</v>
       </c>
       <c r="I18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J18" t="n">
-        <v>31.6</v>
+        <v>3.4</v>
       </c>
       <c r="K18" t="n">
         <v>1.0</v>
@@ -2017,43 +2017,43 @@
         <v>0.0</v>
       </c>
       <c r="N18" t="n">
-        <v>33.0</v>
+        <v>9.0</v>
       </c>
       <c r="O18" t="n">
-        <v>28.0</v>
+        <v>3.0</v>
       </c>
       <c r="P18" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="Q18" t="n">
-        <v>82.0</v>
+        <v>0.0</v>
       </c>
       <c r="R18" t="n">
-        <v>43.0</v>
+        <v>6.0</v>
       </c>
       <c r="S18" t="n">
-        <v>60.0</v>
+        <v>9.0</v>
       </c>
       <c r="T18" t="n">
         <v>0.0</v>
       </c>
       <c r="U18" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="V18" t="n">
         <v>0.0</v>
       </c>
       <c r="W18" t="n">
-        <v>226.0</v>
+        <v>25.0</v>
       </c>
       <c r="X18" t="n">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="Y18" t="n">
-        <v>11.0</v>
+        <v>5.0</v>
       </c>
       <c r="Z18" t="n">
-        <v>45.0</v>
+        <v>61.5</v>
       </c>
     </row>
     <row r="19">
@@ -2061,7 +2061,7 @@
         <v>42</v>
       </c>
       <c r="B19" t="n">
-        <v>1440.0</v>
+        <v>454.0</v>
       </c>
       <c r="C19" t="s">
         <v>73</v>
@@ -2082,10 +2082,10 @@
         <v>129</v>
       </c>
       <c r="I19" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="J19" t="n">
-        <v>2.8</v>
+        <v>32.6</v>
       </c>
       <c r="K19" t="n">
         <v>1.0</v>
@@ -2097,43 +2097,43 @@
         <v>0.0</v>
       </c>
       <c r="N19" t="n">
-        <v>6.0</v>
+        <v>33.0</v>
       </c>
       <c r="O19" t="n">
-        <v>3.0</v>
+        <v>29.0</v>
       </c>
       <c r="P19" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="Q19" t="n">
-        <v>2.0</v>
+        <v>83.0</v>
       </c>
       <c r="R19" t="n">
-        <v>4.0</v>
+        <v>46.0</v>
       </c>
       <c r="S19" t="n">
-        <v>3.0</v>
+        <v>62.0</v>
       </c>
       <c r="T19" t="n">
         <v>0.0</v>
       </c>
       <c r="U19" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="V19" t="n">
         <v>0.0</v>
       </c>
       <c r="W19" t="n">
-        <v>22.0</v>
+        <v>233.0</v>
       </c>
       <c r="X19" t="n">
-        <v>1.0</v>
+        <v>9.0</v>
       </c>
       <c r="Y19" t="n">
-        <v>2.0</v>
+        <v>12.0</v>
       </c>
       <c r="Z19" t="n">
-        <v>33.3</v>
+        <v>42.9</v>
       </c>
     </row>
     <row r="20">
@@ -2141,16 +2141,16 @@
         <v>43</v>
       </c>
       <c r="B20" t="n">
-        <v>1542.0</v>
+        <v>1452.0</v>
       </c>
       <c r="C20" t="s">
         <v>74</v>
       </c>
       <c r="D20" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="E20" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F20" t="s">
         <v>110</v>
@@ -2162,37 +2162,37 @@
         <v>130</v>
       </c>
       <c r="I20" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="J20" t="n">
-        <v>15.7</v>
+        <v>2.8</v>
       </c>
       <c r="K20" t="n">
         <v>1.0</v>
       </c>
       <c r="L20" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="M20" t="n">
         <v>0.0</v>
       </c>
       <c r="N20" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="O20" t="n">
-        <v>10.0</v>
+        <v>3.0</v>
       </c>
       <c r="P20" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="Q20" t="n">
-        <v>21.0</v>
+        <v>2.0</v>
       </c>
       <c r="R20" t="n">
-        <v>17.0</v>
+        <v>4.0</v>
       </c>
       <c r="S20" t="n">
-        <v>18.0</v>
+        <v>3.0</v>
       </c>
       <c r="T20" t="n">
         <v>0.0</v>
@@ -2204,16 +2204,16 @@
         <v>0.0</v>
       </c>
       <c r="W20" t="n">
-        <v>90.0</v>
+        <v>22.0</v>
       </c>
       <c r="X20" t="n">
-        <v>17.0</v>
+        <v>1.0</v>
       </c>
       <c r="Y20" t="n">
-        <v>21.0</v>
+        <v>2.0</v>
       </c>
       <c r="Z20" t="n">
-        <v>44.7</v>
+        <v>33.3</v>
       </c>
     </row>
     <row r="21">
@@ -2221,7 +2221,7 @@
         <v>44</v>
       </c>
       <c r="B21" t="n">
-        <v>1765.0</v>
+        <v>1555.0</v>
       </c>
       <c r="C21" t="s">
         <v>75</v>
@@ -2230,7 +2230,7 @@
         <v>98</v>
       </c>
       <c r="E21" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F21" t="s">
         <v>110</v>
@@ -2242,37 +2242,37 @@
         <v>131</v>
       </c>
       <c r="I21" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="J21" t="n">
-        <v>3.0</v>
+        <v>15.9</v>
       </c>
       <c r="K21" t="n">
         <v>1.0</v>
       </c>
       <c r="L21" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="M21" t="n">
         <v>0.0</v>
       </c>
       <c r="N21" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="O21" t="n">
-        <v>3.0</v>
+        <v>11.0</v>
       </c>
       <c r="P21" t="n">
         <v>1.0</v>
       </c>
       <c r="Q21" t="n">
-        <v>6.0</v>
+        <v>21.0</v>
       </c>
       <c r="R21" t="n">
-        <v>2.0</v>
+        <v>17.0</v>
       </c>
       <c r="S21" t="n">
-        <v>0.0</v>
+        <v>18.0</v>
       </c>
       <c r="T21" t="n">
         <v>0.0</v>
@@ -2284,16 +2284,16 @@
         <v>0.0</v>
       </c>
       <c r="W21" t="n">
-        <v>17.0</v>
+        <v>93.0</v>
       </c>
       <c r="X21" t="n">
-        <v>5.0</v>
+        <v>18.0</v>
       </c>
       <c r="Y21" t="n">
-        <v>8.0</v>
+        <v>21.0</v>
       </c>
       <c r="Z21" t="n">
-        <v>38.5</v>
+        <v>46.2</v>
       </c>
     </row>
     <row r="22">
@@ -2301,7 +2301,7 @@
         <v>45</v>
       </c>
       <c r="B22" t="n">
-        <v>1946.0</v>
+        <v>1781.0</v>
       </c>
       <c r="C22" t="s">
         <v>76</v>
@@ -2322,10 +2322,10 @@
         <v>132</v>
       </c>
       <c r="I22" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="J22" t="n">
-        <v>4.5</v>
+        <v>3.0</v>
       </c>
       <c r="K22" t="n">
         <v>1.0</v>
@@ -2337,22 +2337,22 @@
         <v>0.0</v>
       </c>
       <c r="N22" t="n">
-        <v>7.0</v>
+        <v>4.0</v>
       </c>
       <c r="O22" t="n">
-        <v>9.0</v>
+        <v>3.0</v>
       </c>
       <c r="P22" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="R22" t="n">
         <v>2.0</v>
       </c>
-      <c r="Q22" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="R22" t="n">
-        <v>1.0</v>
-      </c>
       <c r="S22" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="T22" t="n">
         <v>0.0</v>
@@ -2364,16 +2364,16 @@
         <v>0.0</v>
       </c>
       <c r="W22" t="n">
-        <v>12.0</v>
+        <v>17.0</v>
       </c>
       <c r="X22" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="Y22" t="n">
-        <v>13.0</v>
+        <v>8.0</v>
       </c>
       <c r="Z22" t="n">
-        <v>18.8</v>
+        <v>38.5</v>
       </c>
     </row>
     <row r="23">
@@ -2381,7 +2381,7 @@
         <v>46</v>
       </c>
       <c r="B23" t="n">
-        <v>2276.0</v>
+        <v>2298.0</v>
       </c>
       <c r="C23" t="s">
         <v>77</v>
@@ -2402,7 +2402,7 @@
         <v>133</v>
       </c>
       <c r="I23" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="J23" t="n">
         <v>6.1</v>
@@ -2447,13 +2447,13 @@
         <v>26.0</v>
       </c>
       <c r="X23" t="n">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="Y23" t="n">
         <v>17.0</v>
       </c>
       <c r="Z23" t="n">
-        <v>34.6</v>
+        <v>37.0</v>
       </c>
     </row>
     <row r="24">
@@ -2461,7 +2461,7 @@
         <v>47</v>
       </c>
       <c r="B24" t="n">
-        <v>29.0</v>
+        <v>30.0</v>
       </c>
       <c r="C24" t="s">
         <v>78</v>
@@ -2541,7 +2541,7 @@
         <v>48</v>
       </c>
       <c r="B25" t="n">
-        <v>139.0</v>
+        <v>141.0</v>
       </c>
       <c r="C25" t="s">
         <v>79</v>
@@ -2621,7 +2621,7 @@
         <v>49</v>
       </c>
       <c r="B26" t="n">
-        <v>513.0</v>
+        <v>518.0</v>
       </c>
       <c r="C26" t="s">
         <v>80</v>
@@ -2645,7 +2645,7 @@
         <v>145</v>
       </c>
       <c r="J26" t="n">
-        <v>17.5</v>
+        <v>18.3</v>
       </c>
       <c r="K26" t="n">
         <v>0.0</v>
@@ -2666,13 +2666,13 @@
         <v>2.0</v>
       </c>
       <c r="Q26" t="n">
-        <v>64.0</v>
+        <v>67.0</v>
       </c>
       <c r="R26" t="n">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="S26" t="n">
-        <v>14.0</v>
+        <v>15.0</v>
       </c>
       <c r="T26" t="n">
         <v>0.0</v>
@@ -2684,16 +2684,16 @@
         <v>0.0</v>
       </c>
       <c r="W26" t="n">
-        <v>90.0</v>
+        <v>94.0</v>
       </c>
       <c r="X26" t="n">
         <v>1.0</v>
       </c>
       <c r="Y26" t="n">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="Z26" t="n">
-        <v>12.5</v>
+        <v>11.1</v>
       </c>
     </row>
     <row r="27">
@@ -2701,7 +2701,7 @@
         <v>50</v>
       </c>
       <c r="B27" t="n">
-        <v>715.0</v>
+        <v>722.0</v>
       </c>
       <c r="C27" t="s">
         <v>81</v>
@@ -2781,7 +2781,7 @@
         <v>51</v>
       </c>
       <c r="B28" t="n">
-        <v>872.0</v>
+        <v>879.0</v>
       </c>
       <c r="C28" t="s">
         <v>82</v>
@@ -2802,10 +2802,10 @@
         <v>138</v>
       </c>
       <c r="I28" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="J28" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="K28" t="n">
         <v>0.0</v>
@@ -2817,7 +2817,7 @@
         <v>0.0</v>
       </c>
       <c r="N28" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="O28" t="n">
         <v>10.0</v>
@@ -2826,14 +2826,14 @@
         <v>0.0</v>
       </c>
       <c r="Q28" t="n">
-        <v>15.0</v>
+        <v>17.0</v>
       </c>
       <c r="R28" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S28" t="n">
         <v>4.0</v>
       </c>
-      <c r="S28" t="n">
-        <v>2.0</v>
-      </c>
       <c r="T28" t="n">
         <v>0.0</v>
       </c>
@@ -2844,7 +2844,7 @@
         <v>0.0</v>
       </c>
       <c r="W28" t="n">
-        <v>16.0</v>
+        <v>18.0</v>
       </c>
       <c r="X28" t="n">
         <v>0.0</v>
@@ -2861,7 +2861,7 @@
         <v>52</v>
       </c>
       <c r="B29" t="n">
-        <v>1206.0</v>
+        <v>1215.0</v>
       </c>
       <c r="C29" t="s">
         <v>83</v>
@@ -2941,13 +2941,13 @@
         <v>53</v>
       </c>
       <c r="B30" t="n">
-        <v>1476.0</v>
+        <v>1488.0</v>
       </c>
       <c r="C30" t="s">
         <v>84</v>
       </c>
       <c r="D30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E30" t="s">
         <v>109</v>
@@ -2965,7 +2965,7 @@
         <v>159</v>
       </c>
       <c r="J30" t="n">
-        <v>29.0</v>
+        <v>30.0</v>
       </c>
       <c r="K30" t="n">
         <v>0.0</v>
@@ -3021,7 +3021,7 @@
         <v>54</v>
       </c>
       <c r="B31" t="n">
-        <v>2190.0</v>
+        <v>2211.0</v>
       </c>
       <c r="C31" t="s">
         <v>85</v>
@@ -3101,7 +3101,7 @@
         <v>55</v>
       </c>
       <c r="B32" t="n">
-        <v>2313.0</v>
+        <v>2335.0</v>
       </c>
       <c r="C32" t="s">
         <v>86</v>
@@ -3122,7 +3122,7 @@
         <v>142</v>
       </c>
       <c r="I32" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="J32" t="n">
         <v>0.1</v>
@@ -3296,7 +3296,7 @@
         <v>37</v>
       </c>
       <c r="B2" t="n">
-        <v>1386.0</v>
+        <v>1398.0</v>
       </c>
       <c r="C2" t="s">
         <v>68</v>
@@ -3320,7 +3320,7 @@
         <v>151</v>
       </c>
       <c r="J2" t="n">
-        <v>27.0</v>
+        <v>28.0</v>
       </c>
       <c r="K2" t="n">
         <v>26.0</v>
@@ -3329,19 +3329,19 @@
         <v>#N/A</v>
       </c>
       <c r="M2" t="n">
-        <v>24.3</v>
+        <v>24.5</v>
       </c>
       <c r="N2" t="n">
-        <v>16.0</v>
+        <v>17.0</v>
       </c>
       <c r="O2" t="n">
         <v>2.0</v>
       </c>
       <c r="P2" t="n">
-        <v>18.0</v>
+        <v>19.0</v>
       </c>
       <c r="Q2" t="n">
-        <v>15.0</v>
+        <v>16.0</v>
       </c>
       <c r="R2" t="n">
         <v>1.0</v>
@@ -3356,43 +3356,43 @@
         <v>1.0</v>
       </c>
       <c r="V2" t="n">
+        <v>10.3</v>
+      </c>
+      <c r="W2" t="n">
         <v>9.5</v>
       </c>
-      <c r="W2" t="n">
-        <v>8.7</v>
-      </c>
       <c r="X2" t="n">
-        <v>1.7</v>
+        <v>1.9</v>
       </c>
       <c r="Y2" t="n">
-        <v>10.4</v>
+        <v>11.4</v>
       </c>
       <c r="Z2" t="n">
-        <v>18.0</v>
+        <v>21.0</v>
       </c>
       <c r="AA2" t="n">
-        <v>53.0</v>
+        <v>59.0</v>
       </c>
       <c r="AB2" t="n">
-        <v>132.0</v>
+        <v>137.0</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.66</v>
+        <v>0.69</v>
       </c>
       <c r="AD2" t="n">
         <v>0.08</v>
       </c>
       <c r="AE2" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="AG2" t="n">
         <v>0.74</v>
       </c>
-      <c r="AF2" t="n">
-        <v>0.62</v>
-      </c>
-      <c r="AG2" t="n">
-        <v>0.7</v>
-      </c>
       <c r="AH2" t="n">
-        <v>0.39</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="3">
@@ -3400,7 +3400,7 @@
         <v>29</v>
       </c>
       <c r="B3" t="n">
-        <v>1896.0</v>
+        <v>1914.0</v>
       </c>
       <c r="C3" t="s">
         <v>60</v>
@@ -3421,19 +3421,19 @@
         <v>116</v>
       </c>
       <c r="I3" t="s">
-        <v>116</v>
+        <v>146</v>
       </c>
       <c r="J3" t="n">
-        <v>25.0</v>
+        <v>26.0</v>
       </c>
       <c r="K3" t="n">
-        <v>25.0</v>
+        <v>26.0</v>
       </c>
       <c r="L3" t="e">
         <v>#N/A</v>
       </c>
       <c r="M3" t="n">
-        <v>24.3</v>
+        <v>25.3</v>
       </c>
       <c r="N3" t="n">
         <v>4.0</v>
@@ -3472,10 +3472,10 @@
         <v>4.7</v>
       </c>
       <c r="Z3" t="n">
-        <v>14.0</v>
+        <v>15.0</v>
       </c>
       <c r="AA3" t="n">
-        <v>59.0</v>
+        <v>61.0</v>
       </c>
       <c r="AB3" t="n">
         <v>2.0</v>
@@ -3487,30 +3487,30 @@
         <v>0.08</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.25</v>
+        <v>0.24</v>
       </c>
       <c r="AF3" t="n">
         <v>0.16</v>
       </c>
       <c r="AG3" t="n">
-        <v>0.25</v>
+        <v>0.24</v>
       </c>
       <c r="AH3" t="n">
-        <v>0.15</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="B4" t="n">
-        <v>872.0</v>
+        <v>278.0</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="D4" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="E4" t="s">
         <v>106</v>
@@ -3522,31 +3522,31 @@
         <v>111</v>
       </c>
       <c r="H4" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="I4" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="J4" t="n">
-        <v>15.0</v>
+        <v>11.0</v>
       </c>
       <c r="K4" t="n">
-        <v>3.0</v>
+        <v>9.0</v>
       </c>
       <c r="L4" t="n">
-        <v>447.0</v>
+        <v>702.0</v>
       </c>
       <c r="M4" t="n">
-        <v>5.0</v>
+        <v>7.8</v>
       </c>
       <c r="N4" t="n">
         <v>3.0</v>
       </c>
       <c r="O4" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="P4" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="Q4" t="n">
         <v>3.0</v>
@@ -3558,66 +3558,66 @@
         <v>0.0</v>
       </c>
       <c r="T4" t="n">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="U4" t="n">
         <v>0.0</v>
       </c>
       <c r="V4" t="n">
-        <v>0.8</v>
+        <v>1.6</v>
       </c>
       <c r="W4" t="n">
-        <v>0.8</v>
+        <v>1.6</v>
       </c>
       <c r="X4" t="n">
-        <v>0.4</v>
+        <v>2.8</v>
       </c>
       <c r="Y4" t="n">
-        <v>1.3</v>
+        <v>4.4</v>
       </c>
       <c r="Z4" t="n">
-        <v>19.0</v>
+        <v>42.0</v>
       </c>
       <c r="AA4" t="n">
-        <v>8.0</v>
+        <v>28.0</v>
       </c>
       <c r="AB4" t="n">
-        <v>45.0</v>
+        <v>98.0</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.6</v>
+        <v>0.38</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.0</v>
+        <v>0.26</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.6</v>
+        <v>0.64</v>
       </c>
       <c r="AF4" t="n">
-        <v>0.6</v>
+        <v>0.38</v>
       </c>
       <c r="AG4" t="n">
-        <v>0.6</v>
+        <v>0.64</v>
       </c>
       <c r="AH4" t="n">
-        <v>0.17</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="B5" t="n">
-        <v>1881.0</v>
+        <v>879.0</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="D5" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="E5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F5" t="s">
         <v>110</v>
@@ -3626,31 +3626,31 @@
         <v>111</v>
       </c>
       <c r="H5" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="I5" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="J5" t="n">
-        <v>27.0</v>
+        <v>16.0</v>
       </c>
       <c r="K5" t="n">
-        <v>21.0</v>
-      </c>
-      <c r="L5" t="e">
-        <v>#N/A</v>
+        <v>4.0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>537.0</v>
       </c>
       <c r="M5" t="n">
-        <v>19.9</v>
+        <v>6.0</v>
       </c>
       <c r="N5" t="n">
         <v>3.0</v>
       </c>
       <c r="O5" t="n">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="P5" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="Q5" t="n">
         <v>3.0</v>
@@ -3662,66 +3662,66 @@
         <v>0.0</v>
       </c>
       <c r="T5" t="n">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="U5" t="n">
         <v>0.0</v>
       </c>
       <c r="V5" t="n">
-        <v>3.9</v>
+        <v>1.8</v>
       </c>
       <c r="W5" t="n">
-        <v>3.9</v>
+        <v>1.8</v>
       </c>
       <c r="X5" t="n">
-        <v>3.7</v>
+        <v>0.5</v>
       </c>
       <c r="Y5" t="n">
-        <v>7.6</v>
+        <v>2.4</v>
       </c>
       <c r="Z5" t="n">
-        <v>98.0</v>
+        <v>23.0</v>
       </c>
       <c r="AA5" t="n">
-        <v>71.0</v>
+        <v>10.0</v>
       </c>
       <c r="AB5" t="n">
-        <v>222.0</v>
+        <v>54.0</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.15</v>
+        <v>0.5</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.1</v>
+        <v>0.0</v>
       </c>
       <c r="AE5" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="AF5" t="n">
-        <v>0.15</v>
+        <v>0.5</v>
       </c>
       <c r="AG5" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="AH5" t="n">
-        <v>0.19</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B6" t="n">
-        <v>2490.0</v>
+        <v>1899.0</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D6" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E6" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F6" t="s">
         <v>110</v>
@@ -3730,31 +3730,31 @@
         <v>111</v>
       </c>
       <c r="H6" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="I6" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="J6" t="n">
-        <v>24.0</v>
+        <v>28.0</v>
       </c>
       <c r="K6" t="n">
-        <v>24.0</v>
+        <v>21.0</v>
       </c>
       <c r="L6" t="e">
         <v>#N/A</v>
       </c>
       <c r="M6" t="n">
-        <v>22.6</v>
+        <v>20.2</v>
       </c>
       <c r="N6" t="n">
         <v>3.0</v>
       </c>
       <c r="O6" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="P6" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="Q6" t="n">
         <v>3.0</v>
@@ -3766,66 +3766,66 @@
         <v>0.0</v>
       </c>
       <c r="T6" t="n">
-        <v>7.0</v>
+        <v>4.0</v>
       </c>
       <c r="U6" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="V6" t="n">
-        <v>1.8</v>
+        <v>4.0</v>
       </c>
       <c r="W6" t="n">
-        <v>1.8</v>
+        <v>4.0</v>
       </c>
       <c r="X6" t="n">
-        <v>1.0</v>
+        <v>3.8</v>
       </c>
       <c r="Y6" t="n">
-        <v>2.7</v>
+        <v>7.8</v>
       </c>
       <c r="Z6" t="n">
-        <v>31.0</v>
+        <v>104.0</v>
       </c>
       <c r="AA6" t="n">
-        <v>92.0</v>
+        <v>74.0</v>
       </c>
       <c r="AB6" t="n">
-        <v>108.0</v>
+        <v>236.0</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.13</v>
+        <v>0.15</v>
       </c>
       <c r="AD6" t="n">
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="AE6" t="n">
-        <v>0.18</v>
+        <v>0.25</v>
       </c>
       <c r="AF6" t="n">
-        <v>0.13</v>
+        <v>0.15</v>
       </c>
       <c r="AG6" t="n">
-        <v>0.18</v>
+        <v>0.25</v>
       </c>
       <c r="AH6" t="n">
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B7" t="n">
-        <v>275.0</v>
+        <v>2514.0</v>
       </c>
       <c r="C7" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D7" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F7" t="s">
         <v>110</v>
@@ -3834,34 +3834,34 @@
         <v>111</v>
       </c>
       <c r="H7" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="I7" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="J7" t="n">
-        <v>11.0</v>
+        <v>24.0</v>
       </c>
       <c r="K7" t="n">
-        <v>9.0</v>
-      </c>
-      <c r="L7" t="n">
-        <v>702.0</v>
+        <v>24.0</v>
+      </c>
+      <c r="L7" t="e">
+        <v>#N/A</v>
       </c>
       <c r="M7" t="n">
-        <v>7.8</v>
+        <v>22.6</v>
       </c>
       <c r="N7" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="O7" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="P7" t="n">
         <v>4.0</v>
       </c>
       <c r="Q7" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="R7" t="n">
         <v>0.0</v>
@@ -3870,49 +3870,49 @@
         <v>0.0</v>
       </c>
       <c r="T7" t="n">
-        <v>2.0</v>
+        <v>7.0</v>
       </c>
       <c r="U7" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="V7" t="n">
-        <v>1.4</v>
+        <v>1.8</v>
       </c>
       <c r="W7" t="n">
-        <v>1.4</v>
+        <v>1.8</v>
       </c>
       <c r="X7" t="n">
-        <v>2.8</v>
+        <v>1.0</v>
       </c>
       <c r="Y7" t="n">
-        <v>4.2</v>
+        <v>2.7</v>
       </c>
       <c r="Z7" t="n">
-        <v>39.0</v>
+        <v>31.0</v>
       </c>
       <c r="AA7" t="n">
-        <v>27.0</v>
+        <v>97.0</v>
       </c>
       <c r="AB7" t="n">
-        <v>85.0</v>
+        <v>111.0</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.26</v>
+        <v>0.13</v>
       </c>
       <c r="AD7" t="n">
-        <v>0.26</v>
+        <v>0.04</v>
       </c>
       <c r="AE7" t="n">
-        <v>0.51</v>
+        <v>0.18</v>
       </c>
       <c r="AF7" t="n">
-        <v>0.26</v>
+        <v>0.13</v>
       </c>
       <c r="AG7" t="n">
-        <v>0.51</v>
+        <v>0.18</v>
       </c>
       <c r="AH7" t="n">
-        <v>0.18</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="8">
@@ -3920,7 +3920,7 @@
         <v>46</v>
       </c>
       <c r="B8" t="n">
-        <v>2276.0</v>
+        <v>2298.0</v>
       </c>
       <c r="C8" t="s">
         <v>77</v>
@@ -3941,7 +3941,7 @@
         <v>133</v>
       </c>
       <c r="I8" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="J8" t="n">
         <v>20.0</v>
@@ -3980,25 +3980,25 @@
         <v>0.0</v>
       </c>
       <c r="V8" t="n">
-        <v>3.3</v>
+        <v>3.4</v>
       </c>
       <c r="W8" t="n">
-        <v>3.3</v>
+        <v>3.4</v>
       </c>
       <c r="X8" t="n">
-        <v>1.3</v>
+        <v>2.3</v>
       </c>
       <c r="Y8" t="n">
-        <v>4.6</v>
+        <v>5.7</v>
       </c>
       <c r="Z8" t="n">
-        <v>21.0</v>
+        <v>23.0</v>
       </c>
       <c r="AA8" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="AB8" t="n">
-        <v>70.0</v>
+        <v>73.0</v>
       </c>
       <c r="AC8" t="n">
         <v>0.33</v>
@@ -4024,7 +4024,7 @@
         <v>27</v>
       </c>
       <c r="B9" t="n">
-        <v>2545.0</v>
+        <v>2569.0</v>
       </c>
       <c r="C9" t="s">
         <v>58</v>
@@ -4090,16 +4090,16 @@
         <v>2.0</v>
       </c>
       <c r="X9" t="n">
-        <v>1.6</v>
+        <v>1.7</v>
       </c>
       <c r="Y9" t="n">
-        <v>3.6</v>
+        <v>3.7</v>
       </c>
       <c r="Z9" t="n">
-        <v>28.0</v>
+        <v>30.0</v>
       </c>
       <c r="AA9" t="n">
-        <v>141.0</v>
+        <v>146.0</v>
       </c>
       <c r="AB9" t="n">
         <v>64.0</v>
@@ -4128,7 +4128,7 @@
         <v>31</v>
       </c>
       <c r="B10" t="n">
-        <v>91.0</v>
+        <v>92.0</v>
       </c>
       <c r="C10" t="s">
         <v>62</v>
@@ -4149,7 +4149,7 @@
         <v>118</v>
       </c>
       <c r="I10" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J10" t="n">
         <v>8.0</v>
@@ -4229,13 +4229,13 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B11" t="n">
-        <v>450.0</v>
+        <v>454.0</v>
       </c>
       <c r="C11" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D11" t="s">
         <v>89</v>
@@ -4250,22 +4250,22 @@
         <v>111</v>
       </c>
       <c r="H11" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I11" t="s">
         <v>155</v>
       </c>
       <c r="J11" t="n">
-        <v>32.0</v>
+        <v>33.0</v>
       </c>
       <c r="K11" t="n">
-        <v>32.0</v>
+        <v>33.0</v>
       </c>
       <c r="L11" t="e">
         <v>#N/A</v>
       </c>
       <c r="M11" t="n">
-        <v>31.6</v>
+        <v>32.6</v>
       </c>
       <c r="N11" t="n">
         <v>1.0</v>
@@ -4292,40 +4292,40 @@
         <v>0.0</v>
       </c>
       <c r="V11" t="n">
-        <v>2.0</v>
+        <v>2.1</v>
       </c>
       <c r="W11" t="n">
-        <v>2.0</v>
+        <v>2.1</v>
       </c>
       <c r="X11" t="n">
-        <v>5.8</v>
+        <v>5.9</v>
       </c>
       <c r="Y11" t="n">
-        <v>7.8</v>
+        <v>7.9</v>
       </c>
       <c r="Z11" t="n">
-        <v>66.0</v>
+        <v>69.0</v>
       </c>
       <c r="AA11" t="n">
-        <v>261.0</v>
+        <v>276.0</v>
       </c>
       <c r="AB11" t="n">
-        <v>82.0</v>
+        <v>89.0</v>
       </c>
       <c r="AC11" t="n">
         <v>0.03</v>
       </c>
       <c r="AD11" t="n">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="AE11" t="n">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="AF11" t="n">
         <v>0.03</v>
       </c>
       <c r="AG11" t="n">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="AH11" t="n">
         <v>0.06</v>
@@ -4336,7 +4336,7 @@
         <v>49</v>
       </c>
       <c r="B12" t="n">
-        <v>513.0</v>
+        <v>518.0</v>
       </c>
       <c r="C12" t="s">
         <v>80</v>
@@ -4360,25 +4360,25 @@
         <v>145</v>
       </c>
       <c r="J12" t="n">
-        <v>31.0</v>
+        <v>32.0</v>
       </c>
       <c r="K12" t="n">
-        <v>17.0</v>
+        <v>18.0</v>
       </c>
       <c r="L12" t="e">
         <v>#N/A</v>
       </c>
       <c r="M12" t="n">
-        <v>17.5</v>
+        <v>18.3</v>
       </c>
       <c r="N12" t="n">
         <v>1.0</v>
       </c>
       <c r="O12" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="P12" t="n">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="Q12" t="n">
         <v>1.0</v>
@@ -4396,40 +4396,40 @@
         <v>0.0</v>
       </c>
       <c r="V12" t="n">
-        <v>4.5</v>
+        <v>4.8</v>
       </c>
       <c r="W12" t="n">
-        <v>4.5</v>
+        <v>4.8</v>
       </c>
       <c r="X12" t="n">
         <v>4.1</v>
       </c>
       <c r="Y12" t="n">
-        <v>8.6</v>
+        <v>8.9</v>
       </c>
       <c r="Z12" t="n">
-        <v>82.0</v>
+        <v>89.0</v>
       </c>
       <c r="AA12" t="n">
-        <v>123.0</v>
+        <v>133.0</v>
       </c>
       <c r="AB12" t="n">
-        <v>164.0</v>
+        <v>172.0</v>
       </c>
       <c r="AC12" t="n">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="AD12" t="n">
-        <v>0.29</v>
+        <v>0.33</v>
       </c>
       <c r="AE12" t="n">
-        <v>0.34</v>
+        <v>0.38</v>
       </c>
       <c r="AF12" t="n">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="AG12" t="n">
-        <v>0.34</v>
+        <v>0.38</v>
       </c>
       <c r="AH12" t="n">
         <v>0.26</v>
@@ -4440,7 +4440,7 @@
         <v>36</v>
       </c>
       <c r="B13" t="n">
-        <v>1099.0</v>
+        <v>1107.0</v>
       </c>
       <c r="C13" t="s">
         <v>67</v>
@@ -4464,16 +4464,16 @@
         <v>144</v>
       </c>
       <c r="J13" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="K13" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="L13" t="n">
-        <v>532.0</v>
+        <v>607.0</v>
       </c>
       <c r="M13" t="n">
-        <v>5.9</v>
+        <v>6.7</v>
       </c>
       <c r="N13" t="n">
         <v>1.0</v>
@@ -4509,31 +4509,31 @@
         <v>0.4</v>
       </c>
       <c r="Y13" t="n">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="Z13" t="n">
-        <v>19.0</v>
+        <v>20.0</v>
       </c>
       <c r="AA13" t="n">
-        <v>31.0</v>
+        <v>36.0</v>
       </c>
       <c r="AB13" t="n">
-        <v>30.0</v>
+        <v>33.0</v>
       </c>
       <c r="AC13" t="n">
-        <v>0.17</v>
+        <v>0.15</v>
       </c>
       <c r="AD13" t="n">
         <v>0.0</v>
       </c>
       <c r="AE13" t="n">
-        <v>0.17</v>
+        <v>0.15</v>
       </c>
       <c r="AF13" t="n">
-        <v>0.17</v>
+        <v>0.15</v>
       </c>
       <c r="AG13" t="n">
-        <v>0.17</v>
+        <v>0.15</v>
       </c>
       <c r="AH13" t="n">
         <v>0.05</v>
@@ -4544,7 +4544,7 @@
         <v>52</v>
       </c>
       <c r="B14" t="n">
-        <v>1206.0</v>
+        <v>1215.0</v>
       </c>
       <c r="C14" t="s">
         <v>83</v>
@@ -4645,16 +4645,16 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B15" t="n">
-        <v>1542.0</v>
+        <v>1555.0</v>
       </c>
       <c r="C15" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D15" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E15" t="s">
         <v>107</v>
@@ -4666,13 +4666,13 @@
         <v>111</v>
       </c>
       <c r="H15" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="I15" t="s">
         <v>154</v>
       </c>
       <c r="J15" t="n">
-        <v>21.0</v>
+        <v>22.0</v>
       </c>
       <c r="K15" t="n">
         <v>16.0</v>
@@ -4681,7 +4681,7 @@
         <v>#N/A</v>
       </c>
       <c r="M15" t="n">
-        <v>15.7</v>
+        <v>15.9</v>
       </c>
       <c r="N15" t="n">
         <v>1.0</v>
@@ -4708,25 +4708,25 @@
         <v>1.0</v>
       </c>
       <c r="V15" t="n">
-        <v>2.9</v>
+        <v>3.0</v>
       </c>
       <c r="W15" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="X15" t="n">
         <v>2.1</v>
       </c>
-      <c r="X15" t="n">
-        <v>1.5</v>
-      </c>
       <c r="Y15" t="n">
-        <v>3.5</v>
+        <v>4.2</v>
       </c>
       <c r="Z15" t="n">
         <v>26.0</v>
       </c>
       <c r="AA15" t="n">
-        <v>69.0</v>
+        <v>75.0</v>
       </c>
       <c r="AB15" t="n">
-        <v>79.0</v>
+        <v>82.0</v>
       </c>
       <c r="AC15" t="n">
         <v>0.06</v>
@@ -4735,7 +4735,7 @@
         <v>0.25</v>
       </c>
       <c r="AE15" t="n">
-        <v>0.32</v>
+        <v>0.31</v>
       </c>
       <c r="AF15" t="n">
         <v>0.0</v>
@@ -4749,19 +4749,19 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B16" t="n">
-        <v>1946.0</v>
+        <v>1964.0</v>
       </c>
       <c r="C16" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D16" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E16" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F16" t="s">
         <v>110</v>
@@ -4770,22 +4770,22 @@
         <v>111</v>
       </c>
       <c r="H16" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="I16" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J16" t="n">
-        <v>12.0</v>
+        <v>13.0</v>
       </c>
       <c r="K16" t="n">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="L16" t="n">
-        <v>408.0</v>
+        <v>474.0</v>
       </c>
       <c r="M16" t="n">
-        <v>4.5</v>
+        <v>5.3</v>
       </c>
       <c r="N16" t="n">
         <v>1.0</v>
@@ -4806,7 +4806,7 @@
         <v>0.0</v>
       </c>
       <c r="T16" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="U16" t="n">
         <v>0.0</v>
@@ -4827,28 +4827,28 @@
         <v>8.0</v>
       </c>
       <c r="AA16" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="AB16" t="n">
-        <v>31.0</v>
+        <v>33.0</v>
       </c>
       <c r="AC16" t="n">
-        <v>0.22</v>
+        <v>0.19</v>
       </c>
       <c r="AD16" t="n">
         <v>0.0</v>
       </c>
       <c r="AE16" t="n">
-        <v>0.22</v>
+        <v>0.19</v>
       </c>
       <c r="AF16" t="n">
-        <v>0.22</v>
+        <v>0.19</v>
       </c>
       <c r="AG16" t="n">
-        <v>0.22</v>
+        <v>0.19</v>
       </c>
       <c r="AH16" t="n">
-        <v>0.24</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="17">
@@ -4856,7 +4856,7 @@
         <v>47</v>
       </c>
       <c r="B17" t="n">
-        <v>29.0</v>
+        <v>30.0</v>
       </c>
       <c r="C17" t="s">
         <v>78</v>
@@ -4957,13 +4957,13 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B18" t="n">
-        <v>57.0</v>
+        <v>58.0</v>
       </c>
       <c r="C18" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D18" t="s">
         <v>94</v>
@@ -4978,7 +4978,7 @@
         <v>111</v>
       </c>
       <c r="H18" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="I18" t="s">
         <v>154</v>
@@ -5064,7 +5064,7 @@
         <v>48</v>
       </c>
       <c r="B19" t="n">
-        <v>139.0</v>
+        <v>141.0</v>
       </c>
       <c r="C19" t="s">
         <v>79</v>
@@ -5168,7 +5168,7 @@
         <v>33</v>
       </c>
       <c r="B20" t="n">
-        <v>423.0</v>
+        <v>427.0</v>
       </c>
       <c r="C20" t="s">
         <v>64</v>
@@ -5189,19 +5189,19 @@
         <v>120</v>
       </c>
       <c r="I20" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="J20" t="n">
-        <v>22.0</v>
+        <v>23.0</v>
       </c>
       <c r="K20" t="n">
-        <v>20.0</v>
+        <v>21.0</v>
       </c>
       <c r="L20" t="e">
         <v>#N/A</v>
       </c>
       <c r="M20" t="n">
-        <v>20.1</v>
+        <v>21.1</v>
       </c>
       <c r="N20" t="n">
         <v>0.0</v>
@@ -5243,7 +5243,7 @@
         <v>5.0</v>
       </c>
       <c r="AA20" t="n">
-        <v>55.0</v>
+        <v>61.0</v>
       </c>
       <c r="AB20" t="n">
         <v>1.0</v>
@@ -5264,7 +5264,7 @@
         <v>0.0</v>
       </c>
       <c r="AH20" t="n">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="21">
@@ -5272,7 +5272,7 @@
         <v>34</v>
       </c>
       <c r="B21" t="n">
-        <v>692.0</v>
+        <v>699.0</v>
       </c>
       <c r="C21" t="s">
         <v>65</v>
@@ -5293,19 +5293,19 @@
         <v>121</v>
       </c>
       <c r="I21" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="J21" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="K21" t="n">
         <v>4.0</v>
       </c>
       <c r="L21" t="n">
-        <v>347.0</v>
+        <v>358.0</v>
       </c>
       <c r="M21" t="n">
-        <v>3.9</v>
+        <v>4.0</v>
       </c>
       <c r="N21" t="n">
         <v>0.0</v>
@@ -5347,7 +5347,7 @@
         <v>13.0</v>
       </c>
       <c r="AA21" t="n">
-        <v>17.0</v>
+        <v>20.0</v>
       </c>
       <c r="AB21" t="n">
         <v>14.0</v>
@@ -5376,7 +5376,7 @@
         <v>35</v>
       </c>
       <c r="B22" t="n">
-        <v>708.0</v>
+        <v>715.0</v>
       </c>
       <c r="C22" t="s">
         <v>66</v>
@@ -5397,7 +5397,7 @@
         <v>122</v>
       </c>
       <c r="I22" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="J22" t="n">
         <v>10.0</v>
@@ -5480,7 +5480,7 @@
         <v>50</v>
       </c>
       <c r="B23" t="n">
-        <v>715.0</v>
+        <v>722.0</v>
       </c>
       <c r="C23" t="s">
         <v>81</v>
@@ -5584,7 +5584,7 @@
         <v>30</v>
       </c>
       <c r="B24" t="n">
-        <v>1373.0</v>
+        <v>1385.0</v>
       </c>
       <c r="C24" t="s">
         <v>61</v>
@@ -5605,7 +5605,7 @@
         <v>117</v>
       </c>
       <c r="I24" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="J24" t="n">
         <v>17.0</v>
@@ -5685,13 +5685,13 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B25" t="n">
-        <v>1440.0</v>
+        <v>1452.0</v>
       </c>
       <c r="C25" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D25" t="s">
         <v>89</v>
@@ -5706,10 +5706,10 @@
         <v>111</v>
       </c>
       <c r="H25" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I25" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J25" t="n">
         <v>6.0</v>
@@ -5792,13 +5792,13 @@
         <v>53</v>
       </c>
       <c r="B26" t="n">
-        <v>1476.0</v>
+        <v>1488.0</v>
       </c>
       <c r="C26" t="s">
         <v>84</v>
       </c>
       <c r="D26" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E26" t="s">
         <v>109</v>
@@ -5816,16 +5816,16 @@
         <v>159</v>
       </c>
       <c r="J26" t="n">
-        <v>29.0</v>
+        <v>30.0</v>
       </c>
       <c r="K26" t="n">
-        <v>29.0</v>
+        <v>30.0</v>
       </c>
       <c r="L26" t="e">
         <v>#N/A</v>
       </c>
       <c r="M26" t="n">
-        <v>29.0</v>
+        <v>30.0</v>
       </c>
       <c r="N26" t="n">
         <v>0.0</v>
@@ -5867,7 +5867,7 @@
         <v>1.0</v>
       </c>
       <c r="AA26" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="AB26" t="n">
         <v>0.0</v>
@@ -5896,7 +5896,7 @@
         <v>38</v>
       </c>
       <c r="B27" t="n">
-        <v>1492.0</v>
+        <v>1504.0</v>
       </c>
       <c r="C27" t="s">
         <v>69</v>
@@ -6000,7 +6000,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>1620.0</v>
+        <v>1636.0</v>
       </c>
       <c r="C28" t="s">
         <v>57</v>
@@ -6024,16 +6024,16 @@
         <v>143</v>
       </c>
       <c r="J28" t="n">
-        <v>26.0</v>
+        <v>27.0</v>
       </c>
       <c r="K28" t="n">
-        <v>23.0</v>
+        <v>24.0</v>
       </c>
       <c r="L28" t="e">
         <v>#N/A</v>
       </c>
       <c r="M28" t="n">
-        <v>22.7</v>
+        <v>23.7</v>
       </c>
       <c r="N28" t="n">
         <v>0.0</v>
@@ -6054,31 +6054,31 @@
         <v>0.0</v>
       </c>
       <c r="T28" t="n">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="U28" t="n">
         <v>0.0</v>
       </c>
       <c r="V28" t="n">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="W28" t="n">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="X28" t="n">
-        <v>1.6</v>
+        <v>2.2</v>
       </c>
       <c r="Y28" t="n">
-        <v>2.2</v>
+        <v>2.8</v>
       </c>
       <c r="Z28" t="n">
-        <v>29.0</v>
+        <v>32.0</v>
       </c>
       <c r="AA28" t="n">
-        <v>88.0</v>
+        <v>95.0</v>
       </c>
       <c r="AB28" t="n">
-        <v>45.0</v>
+        <v>56.0</v>
       </c>
       <c r="AC28" t="n">
         <v>0.0</v>
@@ -6096,7 +6096,7 @@
         <v>0.13</v>
       </c>
       <c r="AH28" t="n">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="29">
@@ -6104,7 +6104,7 @@
         <v>39</v>
       </c>
       <c r="B29" t="n">
-        <v>1626.0</v>
+        <v>1642.0</v>
       </c>
       <c r="C29" t="s">
         <v>70</v>
@@ -6128,16 +6128,16 @@
         <v>153</v>
       </c>
       <c r="J29" t="n">
-        <v>13.0</v>
+        <v>14.0</v>
       </c>
       <c r="K29" t="n">
-        <v>13.0</v>
+        <v>14.0</v>
       </c>
       <c r="L29" t="e">
         <v>#N/A</v>
       </c>
       <c r="M29" t="n">
-        <v>12.1</v>
+        <v>12.9</v>
       </c>
       <c r="N29" t="n">
         <v>0.0</v>
@@ -6176,13 +6176,13 @@
         <v>0.7</v>
       </c>
       <c r="Z29" t="n">
-        <v>22.0</v>
+        <v>24.0</v>
       </c>
       <c r="AA29" t="n">
-        <v>96.0</v>
+        <v>102.0</v>
       </c>
       <c r="AB29" t="n">
-        <v>15.0</v>
+        <v>16.0</v>
       </c>
       <c r="AC29" t="n">
         <v>0.0</v>
@@ -6205,16 +6205,16 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B30" t="n">
-        <v>1765.0</v>
+        <v>1781.0</v>
       </c>
       <c r="C30" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E30" t="s">
         <v>105</v>
@@ -6226,7 +6226,7 @@
         <v>111</v>
       </c>
       <c r="H30" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I30" t="s">
         <v>156</v>
@@ -6312,7 +6312,7 @@
         <v>54</v>
       </c>
       <c r="B31" t="n">
-        <v>2190.0</v>
+        <v>2211.0</v>
       </c>
       <c r="C31" t="s">
         <v>85</v>
@@ -6416,7 +6416,7 @@
         <v>55</v>
       </c>
       <c r="B32" t="n">
-        <v>2313.0</v>
+        <v>2335.0</v>
       </c>
       <c r="C32" t="s">
         <v>86</v>
@@ -6437,7 +6437,7 @@
         <v>142</v>
       </c>
       <c r="I32" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="J32" t="n">
         <v>1.0</v>

</xml_diff>